<commit_message>
report and user sidebar menu v1
</commit_message>
<xml_diff>
--- a/web/excel/doktor1.xlsx
+++ b/web/excel/doktor1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Web\OpenServer\domains\soglomdi\web\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CFE1D58-BD8E-4D2A-8EF1-501E4B5667E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F08A9E9-534C-4EAC-80D8-5FA0211DB1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="TDSheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TDSheet!$A$4:$W$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TDSheet!$A$4:$X$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>№</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Тўланган сумма</t>
+  </si>
+  <si>
+    <t>Тўлов тури</t>
   </si>
 </sst>
 </file>
@@ -558,10 +561,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="11.4" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -575,16 +578,17 @@
     <col min="7" max="7" width="24.85546875" style="9" customWidth="1"/>
     <col min="8" max="8" width="34.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="24.85546875" style="9" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.85546875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="24.85546875" style="5" customWidth="1"/>
-    <col min="15" max="17" width="24.85546875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="24.85546875" style="5" customWidth="1"/>
-    <col min="19" max="20" width="24.85546875" style="12" customWidth="1"/>
-    <col min="21" max="23" width="24.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" style="9" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="24.85546875" style="5" customWidth="1"/>
+    <col min="16" max="18" width="24.85546875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="24.85546875" style="5" customWidth="1"/>
+    <col min="20" max="21" width="24.85546875" style="12" customWidth="1"/>
+    <col min="22" max="24" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" s="1" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="E1" s="7"/>
@@ -595,12 +599,13 @@
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
-      <c r="N1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="12"/>
+      <c r="M1" s="9"/>
+      <c r="O1" s="5"/>
+      <c r="S1" s="5"/>
       <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
     </row>
-    <row r="2" spans="1:23" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="2" t="s">
@@ -617,21 +622,22 @@
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="10"/>
+      <c r="N2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="6"/>
-      <c r="O2" s="2"/>
+      <c r="O2" s="6"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="13"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="6"/>
       <c r="T2" s="13"/>
-      <c r="U2" s="2"/>
+      <c r="U2" s="13"/>
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:23" s="1" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" s="1" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="E3" s="7"/>
@@ -642,12 +648,13 @@
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
-      <c r="N3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="12"/>
+      <c r="M3" s="9"/>
+      <c r="O3" s="5"/>
+      <c r="S3" s="5"/>
       <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
     </row>
-    <row r="4" spans="1:23" ht="27.6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" ht="27.6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -682,39 +689,42 @@
         <v>23</v>
       </c>
       <c r="L4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="S4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="S4" s="14" t="s">
+      <c r="T4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="T4" s="14" t="s">
+      <c r="U4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="U4" s="4" t="s">
+      <c r="V4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="V4" s="4" t="s">
+      <c r="W4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="W4" s="4" t="s">
+      <c r="X4" s="4" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dok rep fix sum added
</commit_message>
<xml_diff>
--- a/web/excel/doktor1.xlsx
+++ b/web/excel/doktor1.xlsx
@@ -1,29 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Web\OpenServer\domains\soglomdi\web\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\OpenServer\OpenServer\domains\soglomdi\web\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F08A9E9-534C-4EAC-80D8-5FA0211DB1EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="0"/>
   </bookViews>
   <sheets>
     <sheet name="TDSheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TDSheet!$A$4:$X$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TDSheet!$A$4:$Y$4</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>№</t>
   </si>
@@ -98,12 +97,15 @@
   </si>
   <si>
     <t>Тўлов тури</t>
+  </si>
+  <si>
+    <t>Фикс сумма</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
@@ -312,23 +314,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -364,23 +349,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -556,39 +524,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:X4"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="11.4" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="11.45" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" style="9" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="24.85546875" style="9" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" style="9" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.85546875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="24.85546875" style="5" customWidth="1"/>
-    <col min="16" max="18" width="24.85546875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="24.85546875" style="5" customWidth="1"/>
-    <col min="20" max="21" width="24.85546875" style="12" customWidth="1"/>
-    <col min="22" max="24" width="24.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="24.83203125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="34.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="24.83203125" style="9" customWidth="1"/>
+    <col min="12" max="12" width="16.1640625" style="9" customWidth="1"/>
+    <col min="13" max="13" width="14.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.83203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="24.83203125" style="5" customWidth="1"/>
+    <col min="16" max="18" width="24.83203125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="24.83203125" style="5" customWidth="1"/>
+    <col min="20" max="22" width="24.83203125" style="12" customWidth="1"/>
+    <col min="23" max="25" width="24.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" s="1" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="E1" s="7"/>
@@ -604,8 +572,9 @@
       <c r="S1" s="5"/>
       <c r="T1" s="12"/>
       <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
     </row>
-    <row r="2" spans="1:24" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="2" t="s">
@@ -633,11 +602,12 @@
       <c r="S2" s="6"/>
       <c r="T2" s="13"/>
       <c r="U2" s="13"/>
-      <c r="V2" s="2"/>
+      <c r="V2" s="13"/>
       <c r="W2" s="2"/>
       <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
     </row>
-    <row r="3" spans="1:24" s="1" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" s="1" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="E3" s="7"/>
@@ -653,8 +623,9 @@
       <c r="S3" s="5"/>
       <c r="T3" s="12"/>
       <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
     </row>
-    <row r="4" spans="1:24" ht="27.6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -718,13 +689,16 @@
       <c r="U4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="V4" s="4" t="s">
+      <c r="V4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="W4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="W4" s="4" t="s">
+      <c r="X4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="X4" s="4" t="s">
+      <c r="Y4" s="4" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
bp rep rasxod status =2 and doktor1 report sum type fixed
</commit_message>
<xml_diff>
--- a/web/excel/doktor1.xlsx
+++ b/web/excel/doktor1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\OpenServer\OpenServer\domains\soglomdi\web\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Web\OpenServer\domains\soglomdi\web\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69DE298-C287-4A1C-8717-6DF275593D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" tabRatio="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TDSheet" sheetId="1" r:id="rId1"/>
@@ -84,9 +85,6 @@
     <t>Регистратор (филиал)</t>
   </si>
   <si>
-    <t>Саналар</t>
-  </si>
-  <si>
     <t>Пробирка рақами</t>
   </si>
   <si>
@@ -100,12 +98,15 @@
   </si>
   <si>
     <t>Фикс сумма</t>
+  </si>
+  <si>
+    <t>Сана</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
@@ -177,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -219,6 +220,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -314,6 +318,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -349,6 +370,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -524,39 +562,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="11.45" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="11.4" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="24.83203125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="34.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="24.83203125" style="9" customWidth="1"/>
-    <col min="12" max="12" width="16.1640625" style="9" customWidth="1"/>
-    <col min="13" max="13" width="14.83203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.83203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="24.83203125" style="5" customWidth="1"/>
-    <col min="16" max="18" width="24.83203125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="24.83203125" style="5" customWidth="1"/>
-    <col min="20" max="22" width="24.83203125" style="12" customWidth="1"/>
-    <col min="23" max="25" width="24.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="24.85546875" style="9" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" style="9" customWidth="1"/>
+    <col min="12" max="12" width="24.85546875" style="9" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="24.85546875" style="5" customWidth="1"/>
+    <col min="16" max="18" width="24.85546875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="24.85546875" style="5" customWidth="1"/>
+    <col min="20" max="22" width="24.85546875" style="12" customWidth="1"/>
+    <col min="23" max="25" width="24.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" s="1" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="E1" s="7"/>
@@ -574,27 +613,23 @@
       <c r="U1" s="12"/>
       <c r="V1" s="12"/>
     </row>
-    <row r="2" spans="1:25" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" ht="34.799999999999997" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="2" t="s">
-        <v>20</v>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="8"/>
+      <c r="E2" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="F2" s="8"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10" t="s">
-        <v>19</v>
+      <c r="G2" s="15" t="s">
+        <v>7</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
       <c r="K2" s="10"/>
       <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="O2" s="6"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -607,7 +642,7 @@
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
     </row>
-    <row r="3" spans="1:25" s="1" customFormat="1" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" s="1" customFormat="1" ht="9.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="E3" s="7"/>
@@ -625,12 +660,12 @@
       <c r="U3" s="12"/>
       <c r="V3" s="12"/>
     </row>
-    <row r="4" spans="1:25" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" ht="27.6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>1</v>
@@ -660,10 +695,10 @@
         <v>23</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N4" s="4" t="s">
         <v>19</v>
@@ -690,7 +725,7 @@
         <v>15</v>
       </c>
       <c r="V4" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="W4" s="4" t="s">
         <v>17</v>

</xml_diff>